<commit_message>
Update for HWK 16
</commit_message>
<xml_diff>
--- a/Chapter16_17/Chapter16_17.xlsx
+++ b/Chapter16_17/Chapter16_17.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\courses\qmsa\Chapter16_17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F28A2C-82C9-4E5F-AF30-4B663E0E542F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8322666C-8D24-45E3-885B-3E63D2846D3C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Index" sheetId="20" r:id="rId1"/>
+    <sheet name="Chapter 16 - Poverty vs Teenage" sheetId="37" r:id="rId1"/>
     <sheet name="Chapter 16 - Unemployment-Taxes" sheetId="25" r:id="rId2"/>
     <sheet name="Chapter 16 - Guns - Murders" sheetId="26" r:id="rId3"/>
     <sheet name="Chapter 17 - Biomass" sheetId="28" r:id="rId4"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="81">
   <si>
     <t>Georgia</t>
   </si>
@@ -193,99 +193,6 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>Chapter 1</t>
-  </si>
-  <si>
-    <t>Chapter 2</t>
-  </si>
-  <si>
-    <t>Chapter 3</t>
-  </si>
-  <si>
-    <t>Chapter 4</t>
-  </si>
-  <si>
-    <t>Chapter 5</t>
-  </si>
-  <si>
-    <t>Chapter 6</t>
-  </si>
-  <si>
-    <t>Chapter 7</t>
-  </si>
-  <si>
-    <t>Chapter 8</t>
-  </si>
-  <si>
-    <t>Chapter 9</t>
-  </si>
-  <si>
-    <t>Chapter 10</t>
-  </si>
-  <si>
-    <t>Chapter 11</t>
-  </si>
-  <si>
-    <t>Chapter 12</t>
-  </si>
-  <si>
-    <t>Chapter 13</t>
-  </si>
-  <si>
-    <t>Chapter 14</t>
-  </si>
-  <si>
-    <t>Chapter 15</t>
-  </si>
-  <si>
-    <t>Chapter 16</t>
-  </si>
-  <si>
-    <t>Chapter 17</t>
-  </si>
-  <si>
-    <t>Chapter 18</t>
-  </si>
-  <si>
-    <t>Where, Why, What to Do - World Data</t>
-  </si>
-  <si>
-    <t>Data types and classifications - US Data</t>
-  </si>
-  <si>
-    <t>Descriptive Statistics - US Data; MAUP - Snow and Precipitation</t>
-  </si>
-  <si>
-    <t>Descriptive Spatial Statistics - basball teams, Canadian Provinces</t>
-  </si>
-  <si>
-    <t>Probability - Immigration data; Discreet Probability Distributions - NC hurricanes, Tornadoes and Hailstorms in Arkansas</t>
-  </si>
-  <si>
-    <t>Continuous Probability Distributions - NY Snowfall; Probability Mapping - US Temperature</t>
-  </si>
-  <si>
-    <t>Sampling - no data, just examples; Spatial Sampling - NY Soil Types</t>
-  </si>
-  <si>
-    <t>Confidence Interval  Central Limit - Yield Data; Confidence Interval for Stratified Samples - NY Soil types; Point Estimation - Water Meter Data</t>
-  </si>
-  <si>
-    <t>One Sample Difference of Means - USGS Water Use, Wicomico Home Sales</t>
-  </si>
-  <si>
-    <t>Two Sample Difference of Means - Home sales in Wicomico County, Water Use (pool vs. no pool), Brazil Land Uses; Matched Pairs - quartly water use</t>
-  </si>
-  <si>
-    <t>ANOVA - water use for mining, births to teenage mothers, house sales by region of city, yield data and soil</t>
-  </si>
-  <si>
-    <t>No lab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categorical Difference - </t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -304,27 +211,12 @@
     <t>Gun Murders Per 100,000</t>
   </si>
   <si>
-    <t>Correlation - Poverty rate vs. births to teenage mothers; Unemployment vs. State Tax Rate; Gun ownership vs. murders</t>
-  </si>
-  <si>
-    <t>Area Pattern - Join Count: Connecticut obesity; Morans: Connecticut obesity</t>
-  </si>
-  <si>
-    <t>Simple Linear Regression - high school vs. poverty rate; fertilizer vs. yield</t>
-  </si>
-  <si>
-    <t>Point Pattern Nearest Neighbor and Quadrat Analysis - Hurricane Sandy Damage, Connecticut colleges</t>
-  </si>
-  <si>
     <t>Highest Corporate Tax Rate</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiple Regression- fish vs. fisherman, yield vs. OM and other data, </t>
-  </si>
-  <si>
     <t>Biomass (Kg)</t>
   </si>
   <si>
@@ -380,6 +272,12 @@
   </si>
   <si>
     <t>Yield (Bu/Acres)</t>
+  </si>
+  <si>
+    <t>Poverty Rate</t>
+  </si>
+  <si>
+    <t>Births to teenage mothers</t>
   </si>
 </sst>
 </file>
@@ -388,10 +286,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,11 +342,23 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -471,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -488,13 +398,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -519,7 +480,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -530,18 +491,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -555,10 +510,32 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -899,168 +876,589 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BBB002-D332-4CDF-92B7-62870E27FC43}">
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.453125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" style="15"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="16" t="s">
+    <row r="1" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="16"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>95</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="27">
+        <v>13.4</v>
+      </c>
+      <c r="C2" s="26">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="27">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C3" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="27">
+        <v>11.9</v>
+      </c>
+      <c r="C4" s="26">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="27">
+        <v>14.6</v>
+      </c>
+      <c r="C5" s="26">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="27">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C6" s="26">
+        <v>13.200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="27">
+        <v>9.1</v>
+      </c>
+      <c r="C7" s="26">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="27">
+        <v>6.8</v>
+      </c>
+      <c r="C8" s="26">
+        <v>9.7000000000000011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="27">
+        <v>9.5</v>
+      </c>
+      <c r="C9" s="26">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="27">
+        <v>11.7</v>
+      </c>
+      <c r="C10" s="26">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="27">
+        <v>10.1</v>
+      </c>
+      <c r="C11" s="26">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="27">
+        <v>11.7</v>
+      </c>
+      <c r="C12" s="26">
+        <v>14.399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C13" s="26">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="27">
+        <v>8.6</v>
+      </c>
+      <c r="C14" s="26">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="27">
+        <v>9.6</v>
+      </c>
+      <c r="C15" s="26">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="27">
+        <v>11.1</v>
+      </c>
+      <c r="C16" s="26">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C17" s="26">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="27">
+        <v>10.3</v>
+      </c>
+      <c r="C18" s="26">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="27">
+        <v>12.7</v>
+      </c>
+      <c r="C19" s="26">
+        <v>14.799999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="27">
+        <v>13.1</v>
+      </c>
+      <c r="C20" s="26">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="C21" s="26">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C22" s="26">
+        <v>9.7000000000000011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="27">
+        <v>6</v>
+      </c>
+      <c r="C23" s="26">
+        <v>10.100000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="27">
+        <v>10.1</v>
+      </c>
+      <c r="C24" s="26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="27">
+        <v>6.3</v>
+      </c>
+      <c r="C25" s="26">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="27">
+        <v>16.5</v>
+      </c>
+      <c r="C26" s="26">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="27">
+        <v>10.9</v>
+      </c>
+      <c r="C27" s="26">
+        <v>11.600000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="27">
+        <v>10.3</v>
+      </c>
+      <c r="C28" s="26">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C29" s="26">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="27">
+        <v>10.4</v>
+      </c>
+      <c r="C30" s="26">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="27">
+        <v>5.7</v>
+      </c>
+      <c r="C31" s="26">
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="27">
+        <v>5.9</v>
+      </c>
+      <c r="C32" s="26">
+        <v>6.8000000000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="27">
+        <v>15.5</v>
+      </c>
+      <c r="C33" s="26">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27">
+        <v>6.7</v>
+      </c>
+      <c r="C34" s="26">
+        <v>14.499999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="27">
+        <v>11.3</v>
+      </c>
+      <c r="C35" s="26">
+        <v>13.100000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="27">
+        <v>7.4</v>
+      </c>
+      <c r="C36" s="26">
+        <v>11.200000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="27">
+        <v>10.8</v>
+      </c>
+      <c r="C37" s="26">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="27">
+        <v>13.8</v>
+      </c>
+      <c r="C38" s="26">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C39" s="26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="27">
+        <v>8.9</v>
+      </c>
+      <c r="C40" s="26">
+        <v>11.200000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C41" s="26">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="27">
+        <v>12.8</v>
+      </c>
+      <c r="C42" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="27">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C43" s="26">
+        <v>11.799999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="27">
+        <v>12.8</v>
+      </c>
+      <c r="C44" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="27">
+        <v>13.3</v>
+      </c>
+      <c r="C45" s="26">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="27">
+        <v>6.3</v>
+      </c>
+      <c r="C46" s="26">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="27">
+        <v>6.5</v>
+      </c>
+      <c r="C47" s="26">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="27">
+        <v>7.9</v>
+      </c>
+      <c r="C48" s="26">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="C49" s="26">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="27">
+        <v>13.5</v>
+      </c>
+      <c r="C50" s="26">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C51" s="26">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="28">
+        <v>10.4</v>
+      </c>
+      <c r="C52" s="29">
+        <v>10.6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1068,32 +1466,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -1107,7 +1505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -1121,7 +1519,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
@@ -1149,7 +1547,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1561,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1575,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1191,7 +1589,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1603,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -1219,7 +1617,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1233,7 +1631,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
@@ -1247,7 +1645,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -1261,7 +1659,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -1275,7 +1673,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>15</v>
       </c>
@@ -1289,7 +1687,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>16</v>
       </c>
@@ -1303,7 +1701,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>17</v>
       </c>
@@ -1317,7 +1715,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>18</v>
       </c>
@@ -1331,7 +1729,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>19</v>
       </c>
@@ -1345,7 +1743,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>20</v>
       </c>
@@ -1359,7 +1757,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>21</v>
       </c>
@@ -1373,7 +1771,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
@@ -1387,7 +1785,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>23</v>
       </c>
@@ -1401,7 +1799,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
@@ -1415,7 +1813,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
@@ -1429,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
@@ -1443,7 +1841,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>27</v>
       </c>
@@ -1457,7 +1855,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>28</v>
       </c>
@@ -1471,7 +1869,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>29</v>
       </c>
@@ -1485,7 +1883,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
@@ -1499,7 +1897,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>31</v>
       </c>
@@ -1513,7 +1911,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
@@ -1527,7 +1925,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>33</v>
       </c>
@@ -1541,7 +1939,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>34</v>
       </c>
@@ -1555,7 +1953,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>35</v>
       </c>
@@ -1569,7 +1967,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>36</v>
       </c>
@@ -1577,15 +1975,15 @@
         <v>5.3920000000000003</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D36" s="3">
         <v>5.7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="B37" s="11">
         <v>5.25</v>
@@ -1597,7 +1995,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>38</v>
       </c>
@@ -1611,7 +2009,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>39</v>
       </c>
@@ -1625,7 +2023,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>40</v>
       </c>
@@ -1639,7 +2037,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>41</v>
       </c>
@@ -1653,7 +2051,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>42</v>
       </c>
@@ -1667,7 +2065,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>43</v>
       </c>
@@ -1681,7 +2079,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +2093,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>45</v>
       </c>
@@ -1709,7 +2107,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>46</v>
       </c>
@@ -1723,7 +2121,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>47</v>
       </c>
@@ -1737,7 +2135,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>48</v>
       </c>
@@ -1745,13 +2143,13 @@
         <v>0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D48" s="3">
         <v>5.6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>49</v>
       </c>
@@ -1765,7 +2163,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>50</v>
       </c>
@@ -1779,7 +2177,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>51</v>
       </c>
@@ -1807,24 +2205,24 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.26953125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1835,7 +2233,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +2244,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1857,7 +2255,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1868,7 +2266,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1879,7 +2277,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +2288,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1901,7 +2299,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1912,7 +2310,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1923,7 +2321,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1934,7 +2332,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +2343,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1956,7 +2354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1967,7 +2365,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1978,7 +2376,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1989,7 +2387,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2000,7 +2398,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2011,7 +2409,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2022,7 +2420,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2033,7 +2431,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2044,7 +2442,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2055,7 +2453,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2066,7 +2464,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2077,7 +2475,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2088,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2099,7 +2497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2110,7 +2508,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2121,7 +2519,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2132,7 +2530,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2143,7 +2541,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2154,7 +2552,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2165,7 +2563,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2176,7 +2574,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2187,7 +2585,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2198,7 +2596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2209,7 +2607,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2220,7 +2618,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2231,7 +2629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2242,7 +2640,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2253,7 +2651,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2264,7 +2662,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2275,7 +2673,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2286,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2297,7 +2695,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2308,7 +2706,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2319,7 +2717,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2330,7 +2728,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2341,7 +2739,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2352,7 +2750,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2363,7 +2761,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2374,7 +2772,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2398,335 +2796,335 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="52" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="18">
+    <row r="1" spans="1:3" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
         <v>3.7</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="16">
         <v>5</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="18">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>8.5</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>14.8</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="18">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>20.3</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>166.5</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="18">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
         <v>24</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>241</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="18">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>31</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>417</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="18">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
         <v>41</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>510.9</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="18">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>23.2</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="16">
         <v>343.1</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="18">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>23.5</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <v>446.7</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="18">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>23.8</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="16">
         <v>243.3</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="18">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <v>24.2</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>367.5</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="18">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>31.8</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <v>454.4</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="18">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>15.2</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="16">
         <v>52</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="18">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>17.100000000000001</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>27.1</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="18">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>18.399999999999999</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <v>69.900000000000006</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="18">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>23.2</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <v>202.6</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="18">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>29.6</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>414</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
         <v>30.2</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <v>394.8</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="18">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>34.700000000000003</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>550.79999999999995</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="18">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
         <v>10.8</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>32.6</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="18">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
         <v>18.7</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="16">
         <v>92.3</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="18">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>21.6</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="16">
         <v>191.4</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="18">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
         <v>39.200000000000003</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="16">
         <v>407.7</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="18">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
         <v>29.9</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="16">
         <v>225.3</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="18">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
         <v>30.2</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="16">
         <v>378.9</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="18">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
         <v>17.100000000000001</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>81.8</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="18">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
         <v>34</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <v>709.7</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="18">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
         <v>19.399999999999999</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="16">
         <v>113.9</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="18">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
         <v>14.6</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="16">
         <v>51.2</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="18">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
         <v>12.4</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="16">
         <v>64.099999999999994</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="16">
         <v>2</v>
       </c>
     </row>
@@ -2744,25 +3142,25 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="19">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
         <v>41913.697916666664</v>
       </c>
       <c r="B2" s="6">
@@ -2772,8 +3170,8 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="19">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
         <v>41913.802083333336</v>
       </c>
       <c r="B3" s="6">
@@ -2783,8 +3181,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
         <v>41913.90625</v>
       </c>
       <c r="B4" s="6">
@@ -2794,8 +3192,8 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="19">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>41914.010416666664</v>
       </c>
       <c r="B5" s="6">
@@ -2805,8 +3203,8 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>41914.114583333336</v>
       </c>
       <c r="B6" s="6">
@@ -2816,8 +3214,8 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>41914.21875</v>
       </c>
       <c r="B7" s="6">
@@ -2827,8 +3225,8 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="19">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>41914.322916666664</v>
       </c>
       <c r="B8" s="6">
@@ -2838,8 +3236,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
         <v>41914.427083333336</v>
       </c>
       <c r="B9" s="6">
@@ -2849,8 +3247,8 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="19">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
         <v>41914.53125</v>
       </c>
       <c r="B10" s="6">
@@ -2860,8 +3258,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="19">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>41914.635416666664</v>
       </c>
       <c r="B11" s="6">
@@ -2871,8 +3269,8 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="19">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>41914.739583333336</v>
       </c>
       <c r="B12" s="6">
@@ -2882,8 +3280,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="19">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>41914.84375</v>
       </c>
       <c r="B13" s="6">
@@ -2893,8 +3291,8 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="19">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <v>41914.947916666664</v>
       </c>
       <c r="B14" s="6">
@@ -2904,8 +3302,8 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="19">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
         <v>41915.052083333336</v>
       </c>
       <c r="B15" s="6">
@@ -2915,8 +3313,8 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="19">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
         <v>41915.15625</v>
       </c>
       <c r="B16" s="6">
@@ -2926,8 +3324,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="19">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
         <v>41915.260416666664</v>
       </c>
       <c r="B17" s="6">
@@ -2937,8 +3335,8 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="19">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
         <v>41915.364583333336</v>
       </c>
       <c r="B18" s="6">
@@ -2948,8 +3346,8 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
         <v>41915.46875</v>
       </c>
       <c r="B19" s="6">
@@ -2959,8 +3357,8 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="19">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
         <v>41915.572916666664</v>
       </c>
       <c r="B20" s="6">
@@ -2970,8 +3368,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="19">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
         <v>41915.677083333336</v>
       </c>
       <c r="B21" s="6">
@@ -2981,8 +3379,8 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="19">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
         <v>41915.78125</v>
       </c>
       <c r="B22" s="6">
@@ -2992,8 +3390,8 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="19">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
         <v>41915.885416666664</v>
       </c>
       <c r="B23" s="6">
@@ -3003,8 +3401,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="19">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
         <v>41915.989583333336</v>
       </c>
       <c r="B24" s="6">
@@ -3014,8 +3412,8 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="19">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
         <v>41916.09375</v>
       </c>
       <c r="B25" s="6">
@@ -3025,8 +3423,8 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="19">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
         <v>41916.197916666664</v>
       </c>
       <c r="B26" s="6">
@@ -3036,8 +3434,8 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="19">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
         <v>41916.302083333336</v>
       </c>
       <c r="B27" s="6">
@@ -3047,8 +3445,8 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="19">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
         <v>41916.40625</v>
       </c>
       <c r="B28" s="6">
@@ -3058,8 +3456,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="19">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
         <v>41916.510416666664</v>
       </c>
       <c r="B29" s="6">
@@ -3069,8 +3467,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="19">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
         <v>41916.614583333336</v>
       </c>
       <c r="B30" s="6">
@@ -3080,8 +3478,8 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="19">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
         <v>41916.71875</v>
       </c>
       <c r="B31" s="6">
@@ -3091,8 +3489,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="19">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
         <v>41916.822916666664</v>
       </c>
       <c r="B32" s="6">
@@ -3102,8 +3500,8 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="19">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
         <v>41916.927083333336</v>
       </c>
       <c r="B33" s="6">
@@ -3113,8 +3511,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="19">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
         <v>41917.03125</v>
       </c>
       <c r="B34" s="6">
@@ -3124,8 +3522,8 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="19">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
         <v>41917.135416666664</v>
       </c>
       <c r="B35" s="6">
@@ -3135,8 +3533,8 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="19">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
         <v>41917.239583333336</v>
       </c>
       <c r="B36" s="6">
@@ -3146,8 +3544,8 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="19">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
         <v>41917.34375</v>
       </c>
       <c r="B37" s="6">
@@ -3157,8 +3555,8 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="19">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
         <v>41917.447916666664</v>
       </c>
       <c r="B38" s="6">
@@ -3168,8 +3566,8 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="19">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
         <v>41917.552083333336</v>
       </c>
       <c r="B39" s="6">
@@ -3179,8 +3577,8 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="19">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
         <v>41917.65625</v>
       </c>
       <c r="B40" s="6">
@@ -3190,8 +3588,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="19">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
         <v>41917.760416666664</v>
       </c>
       <c r="B41" s="6">
@@ -3201,8 +3599,8 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="19">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
         <v>41917.864583333336</v>
       </c>
       <c r="B42" s="6">
@@ -3212,8 +3610,8 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="19">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
         <v>41917.96875</v>
       </c>
       <c r="B43" s="6">
@@ -3223,8 +3621,8 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="19">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
         <v>41918.072916666664</v>
       </c>
       <c r="B44" s="6">
@@ -3234,8 +3632,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="19">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
         <v>41918.177083333336</v>
       </c>
       <c r="B45" s="6">
@@ -3245,8 +3643,8 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="19">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
         <v>41918.28125</v>
       </c>
       <c r="B46" s="6">
@@ -3269,335 +3667,335 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" style="3"/>
-    <col min="3" max="3" width="15.90625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>240450001002</v>
       </c>
       <c r="B2" s="3">
         <v>8</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="18">
         <v>43.3689503456945</v>
       </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>240450001003</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="18">
         <v>69.2456479690522</v>
       </c>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>240450001005</v>
       </c>
       <c r="B4" s="3">
         <v>30</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="18">
         <v>33.019502353732399</v>
       </c>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>240450002001</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <v>64.240102171136698</v>
       </c>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>240450002002</v>
       </c>
       <c r="B6" s="3">
         <v>14</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="18">
         <v>46.102150537634401</v>
       </c>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>240450003001</v>
       </c>
       <c r="B7" s="3">
         <v>16</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="18">
         <v>10.646387832699599</v>
       </c>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>240450003002</v>
       </c>
       <c r="B8" s="3">
         <v>14</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <v>15.880893300248101</v>
       </c>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>240450004001</v>
       </c>
       <c r="B9" s="3">
         <v>18</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="18">
         <v>29.747899159663898</v>
       </c>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>240450004002</v>
       </c>
       <c r="B10" s="3">
         <v>10</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="18">
         <v>61.019490254872601</v>
       </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>240450004005</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="18">
         <v>53.536977491961402</v>
       </c>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>240450005001</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="18">
         <v>56.331877729257599</v>
       </c>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>240450005002</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="18">
         <v>62.170385395537494</v>
       </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13" s="19"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>240450005003</v>
       </c>
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="18">
         <v>63.047285464098103</v>
       </c>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>240450101101</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="18">
         <v>72.307692307692292</v>
       </c>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>240450101103</v>
       </c>
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="18">
         <v>98.765432098765402</v>
       </c>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E16" s="19"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>240450101105</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="18">
         <v>87.089947089947088</v>
       </c>
-      <c r="E17" s="21"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>240450101201</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="18">
         <v>58.554342173686905</v>
       </c>
-      <c r="E18" s="21"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>240450102003</v>
       </c>
       <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="18">
         <v>28.828828828828801</v>
       </c>
-      <c r="E19" s="21"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>240450102005</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="18">
         <v>32.150776053215104</v>
       </c>
-      <c r="E20" s="21"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" s="19"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>240450104003</v>
       </c>
       <c r="B21" s="3">
         <v>5</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="18">
         <v>81.869290231904401</v>
       </c>
-      <c r="E21" s="21"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>240450104004</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="18">
         <v>71.6591928251121</v>
       </c>
-      <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>240450105001</v>
       </c>
       <c r="B23" s="3">
         <v>2</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="18">
         <v>52.572347266881003</v>
       </c>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>240450105004</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="18">
         <v>75.390890550645793</v>
       </c>
-      <c r="E24" s="21"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>240450105005</v>
       </c>
       <c r="B25" s="3">
         <v>2</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="18">
         <v>86.792452830188708</v>
       </c>
-      <c r="E25" s="21"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>240450106102</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="18">
         <v>88.156424581005595</v>
       </c>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>240450107206</v>
       </c>
       <c r="B27" s="3">
         <v>4</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="18">
         <v>66.6666666666667</v>
       </c>
-      <c r="E27" s="21"/>
+      <c r="E27" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3613,30 +4011,30 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.6328125" style="3"/>
-    <col min="5" max="5" width="11.54296875" style="3" customWidth="1"/>
+    <col min="1" max="4" width="8.5703125" style="3"/>
+    <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2.4</v>
       </c>
@@ -3653,7 +4051,7 @@
         <v>138.161194029851</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2.4</v>
       </c>
@@ -3670,7 +4068,7 @@
         <v>138.919858156028</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2.9</v>
       </c>
@@ -3687,7 +4085,7 @@
         <v>133.37375</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3.1</v>
       </c>
@@ -3704,7 +4102,7 @@
         <v>136.16882352941201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3.2</v>
       </c>
@@ -3721,7 +4119,7 @@
         <v>116.363870967742</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3.2</v>
       </c>
@@ -3738,7 +4136,7 @@
         <v>146.437426900585</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>3.3</v>
       </c>
@@ -3755,7 +4153,7 @@
         <v>134.213496932515</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3.5</v>
       </c>
@@ -3772,7 +4170,7 @@
         <v>139.71388888888899</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>3.5</v>
       </c>
@@ -3789,7 +4187,7 @@
         <v>104.25757575757601</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>3.6</v>
       </c>
@@ -3806,7 +4204,7 @@
         <v>136.970909090909</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>3.6</v>
       </c>
@@ -3823,7 +4221,7 @@
         <v>141.852866242038</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>3.7</v>
       </c>
@@ -3840,7 +4238,7 @@
         <v>148.14900662251699</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>3.8</v>
       </c>
@@ -3857,7 +4255,7 @@
         <v>140.045517241379</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>3.8</v>
       </c>
@@ -3874,7 +4272,7 @@
         <v>143.03860759493699</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -3891,7 +4289,7 @@
         <v>147.91140939597301</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>4.0999999999999996</v>
       </c>
@@ -3908,7 +4306,7 @@
         <v>139.16050955413999</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>4.4000000000000004</v>
       </c>
@@ -3925,7 +4323,7 @@
         <v>81.498666666666693</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>4.5</v>
       </c>
@@ -3942,7 +4340,7 @@
         <v>143.94932432432401</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>4.5999999999999996</v>
       </c>
@@ -3959,7 +4357,7 @@
         <v>117.51858974359</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>4.5999999999999996</v>
       </c>
@@ -3976,7 +4374,7 @@
         <v>80.583448275862096</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>4.7</v>
       </c>
@@ -3993,7 +4391,7 @@
         <v>102.166197183099</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>4.7</v>
       </c>
@@ -4010,7 +4408,7 @@
         <v>124.363535911602</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>4.8</v>
       </c>
@@ -4027,7 +4425,7 @@
         <v>118.632530120482</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>5.4</v>
       </c>
@@ -4058,29 +4456,29 @@
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>500000</v>
       </c>
@@ -4100,7 +4498,7 @@
         <v>0.377769984719595</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>400000</v>
       </c>
@@ -4120,7 +4518,7 @@
         <v>0.43454464921309899</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1750000</v>
       </c>
@@ -4136,11 +4534,11 @@
       <c r="E4">
         <v>589337.82258064498</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="20">
         <v>1.9472810556396901E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>265900</v>
       </c>
@@ -4160,7 +4558,7 @@
         <v>0.28045125477202398</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>350000</v>
       </c>
@@ -4180,7 +4578,7 @@
         <v>0.25286139252367601</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>237000</v>
       </c>
@@ -4200,7 +4598,7 @@
         <v>0.44599912496598598</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>685000</v>
       </c>
@@ -4220,7 +4618,7 @@
         <v>0.60553965273676003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>484472</v>
       </c>
@@ -4240,7 +4638,7 @@
         <v>0.25393899800597702</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>465000</v>
       </c>
@@ -4260,7 +4658,7 @@
         <v>0.57820139171020601</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>425000</v>
       </c>
@@ -4280,7 +4678,7 @@
         <v>0.419204829815774</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>560000</v>
       </c>
@@ -4300,7 +4698,7 @@
         <v>0.25424389402022102</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>445000</v>
       </c>
@@ -4320,7 +4718,7 @@
         <v>0.13585567470114299</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>860000</v>
       </c>
@@ -4336,11 +4734,11 @@
       <c r="E14">
         <v>475795.07462686597</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <v>8.2891204152846398E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1025000</v>
       </c>
@@ -4356,11 +4754,11 @@
       <c r="E15">
         <v>742245.45454545505</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="20">
         <v>3.2971518634760603E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>262000</v>
       </c>
@@ -4380,7 +4778,7 @@
         <v>0.63731082904033498</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>518721</v>
       </c>
@@ -4400,7 +4798,7 @@
         <v>0.277474684637943</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>382050</v>
       </c>
@@ -4420,7 +4818,7 @@
         <v>0.13476716833316199</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>783782</v>
       </c>
@@ -4440,7 +4838,7 @@
         <v>0.209990486053652</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>275000</v>
       </c>
@@ -4460,7 +4858,7 @@
         <v>0.36250418891948899</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1470000</v>
       </c>
@@ -4480,7 +4878,7 @@
         <v>0.115256976892799</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>575000</v>
       </c>
@@ -4500,7 +4898,7 @@
         <v>0.13861103699148</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1750125</v>
       </c>
@@ -4516,11 +4914,11 @@
       <c r="E23">
         <v>625780.28301886795</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="20">
         <v>2.2974720305802099E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>515000</v>
       </c>
@@ -4540,7 +4938,7 @@
         <v>0.39270629205708601</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>150000</v>
       </c>
@@ -4560,7 +4958,7 @@
         <v>0.122854267560951</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>327000</v>
       </c>
@@ -4580,7 +4978,7 @@
         <v>0.56781504390218995</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>493000</v>
       </c>
@@ -4600,7 +4998,7 @@
         <v>0.66012803128828101</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>609475</v>
       </c>
@@ -4620,7 +5018,7 @@
         <v>0.284493779929547</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>757700</v>
       </c>
@@ -4640,7 +5038,7 @@
         <v>0.24417551359210701</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>209900</v>
       </c>
@@ -4660,7 +5058,7 @@
         <v>0.93301132730527003</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>775000</v>
       </c>
@@ -4680,7 +5078,7 @@
         <v>0.305984594320452</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>535000</v>
       </c>
@@ -4700,7 +5098,7 @@
         <v>0.183656693238229</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>256000</v>
       </c>
@@ -4720,7 +5118,7 @@
         <v>0.28053753231606499</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>212500</v>
       </c>
@@ -4740,7 +5138,7 @@
         <v>0.386133743349518</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>511000</v>
       </c>
@@ -4760,7 +5158,7 @@
         <v>0.238268738577988</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>285000</v>
       </c>
@@ -4780,7 +5178,7 @@
         <v>0.63712796511485403</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>649950</v>
       </c>
@@ -4800,7 +5198,7 @@
         <v>0.192455717408024</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>600000</v>
       </c>
@@ -4820,7 +5218,7 @@
         <v>0.178581827910472</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>232900</v>
       </c>
@@ -4840,7 +5238,7 @@
         <v>0.47607697155678003</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>485000</v>
       </c>
@@ -4860,7 +5258,7 @@
         <v>9.7310997046145001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>350000</v>
       </c>

</xml_diff>